<commit_message>
feat/ Added flight feature with skycanner API. refactor/ Refactored schema to accept departure city and airport code.
</commit_message>
<xml_diff>
--- a/travelapp_spreadsheet.xlsx
+++ b/travelapp_spreadsheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>city</t>
   </si>
@@ -37,79 +37,142 @@
     <t>group_relationship</t>
   </si>
   <si>
+    <t>airport_code</t>
+  </si>
+  <si>
     <t>Montreal, Canada</t>
   </si>
   <si>
+    <t>YUL-sky</t>
+  </si>
+  <si>
     <t>Vancouver, Canada</t>
   </si>
   <si>
+    <t>YVR-sky</t>
+  </si>
+  <si>
     <t>Tulum, Mexico</t>
   </si>
   <si>
+    <t>CUN-sky</t>
+  </si>
+  <si>
     <t>Cancun, Mexico</t>
   </si>
   <si>
-    <t>Mexico City, Mexico</t>
-  </si>
-  <si>
     <t>San Fransisco, CA</t>
   </si>
   <si>
+    <t>SFO-sky</t>
+  </si>
+  <si>
     <t>Seattle, WA</t>
   </si>
   <si>
+    <t>SEA-sky</t>
+  </si>
+  <si>
     <t>Park City, UT</t>
   </si>
   <si>
+    <t>SLC-sky</t>
+  </si>
+  <si>
     <t>Aspen, CO</t>
   </si>
   <si>
+    <t>DEN-sky</t>
+  </si>
+  <si>
     <t>Chicago, IL</t>
   </si>
   <si>
+    <t>ORD-sky</t>
+  </si>
+  <si>
     <t>New York City, NY</t>
   </si>
   <si>
+    <t>JFK-sky</t>
+  </si>
+  <si>
     <t>Miami, FL</t>
   </si>
   <si>
+    <t>MIA-sky</t>
+  </si>
+  <si>
     <t>Los Angeles, CA</t>
   </si>
   <si>
+    <t>LAX-sky</t>
+  </si>
+  <si>
     <t>Nashville, TN</t>
   </si>
   <si>
+    <t>BNA-sky</t>
+  </si>
+  <si>
     <t>Austin, TX</t>
   </si>
   <si>
+    <t>AUS-sky</t>
+  </si>
+  <si>
     <t>Charleston, SC</t>
   </si>
   <si>
+    <t>CHS-sky</t>
+  </si>
+  <si>
     <t>Savannah, GA</t>
   </si>
   <si>
+    <t>ATL-sky</t>
+  </si>
+  <si>
     <t>Boston, MA</t>
   </si>
   <si>
+    <t>BOS-sky</t>
+  </si>
+  <si>
     <t>Washington, D.C.</t>
   </si>
   <si>
+    <t>DCA-sky</t>
+  </si>
+  <si>
     <t>New Orleans, LA</t>
   </si>
   <si>
-    <t>San Juan, Puerto Rico</t>
+    <t>MSY-sky</t>
   </si>
   <si>
     <t>Philadelphia, PA</t>
   </si>
   <si>
-    <t>Scranton, PA</t>
+    <t>PHL-sky</t>
   </si>
   <si>
     <t>San Diego, CA</t>
   </si>
   <si>
+    <t>SAN-sky</t>
+  </si>
+  <si>
     <t>Orlando, FL</t>
+  </si>
+  <si>
+    <t>MCO-sky</t>
+  </si>
+  <si>
+    <t>Portland, OR</t>
+  </si>
+  <si>
+    <t>PDX-sky</t>
   </si>
 </sst>
 </file>
@@ -372,8 +435,8 @@
     <col customWidth="1" min="3" max="4" width="21.71"/>
     <col customWidth="1" min="5" max="5" width="13.57"/>
     <col customWidth="1" min="6" max="6" width="20.14"/>
-    <col customWidth="1" min="7" max="7" width="37.71"/>
-    <col customWidth="1" min="8" max="8" width="14.0"/>
+    <col customWidth="1" min="7" max="7" width="24.43"/>
+    <col customWidth="1" min="8" max="8" width="16.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -401,10 +464,14 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1">
         <v>40.0</v>
@@ -426,11 +493,14 @@
       </c>
       <c r="H2" s="1">
         <v>80.0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1">
         <v>40.0</v>
@@ -452,11 +522,14 @@
       </c>
       <c r="H3" s="1">
         <v>80.0</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1">
         <v>100.0</v>
@@ -478,11 +551,14 @@
       </c>
       <c r="H4" s="1">
         <v>80.0</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1">
         <v>100.0</v>
@@ -504,43 +580,49 @@
       </c>
       <c r="H5" s="1">
         <v>40.0</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1">
-        <v>100.0</v>
+        <v>60.0</v>
       </c>
       <c r="C6" s="1">
-        <v>60.0</v>
+        <v>100.0</v>
       </c>
       <c r="D6" s="1">
         <v>60.0</v>
       </c>
       <c r="E6" s="1">
-        <v>100.0</v>
+        <v>60.0</v>
       </c>
       <c r="F6" s="1">
-        <v>100.0</v>
+        <v>20.0</v>
       </c>
       <c r="G6" s="1">
-        <v>60.0</v>
+        <v>80.0</v>
       </c>
       <c r="H6" s="1">
-        <v>60.0</v>
+        <v>80.0</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1">
         <v>60.0</v>
       </c>
       <c r="C7" s="1">
-        <v>100.0</v>
+        <v>80.0</v>
       </c>
       <c r="D7" s="1">
         <v>60.0</v>
@@ -552,24 +634,27 @@
         <v>20.0</v>
       </c>
       <c r="G7" s="1">
-        <v>80.0</v>
+        <v>60.0</v>
       </c>
       <c r="H7" s="1">
         <v>80.0</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1">
-        <v>60.0</v>
+        <v>40.0</v>
       </c>
       <c r="C8" s="1">
         <v>80.0</v>
       </c>
       <c r="D8" s="1">
-        <v>60.0</v>
+        <v>100.0</v>
       </c>
       <c r="E8" s="1">
         <v>60.0</v>
@@ -582,11 +667,14 @@
       </c>
       <c r="H8" s="1">
         <v>80.0</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1">
         <v>40.0</v>
@@ -608,11 +696,14 @@
       </c>
       <c r="H9" s="1">
         <v>80.0</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1">
         <v>40.0</v>
@@ -621,10 +712,10 @@
         <v>80.0</v>
       </c>
       <c r="D10" s="1">
-        <v>100.0</v>
+        <v>20.0</v>
       </c>
       <c r="E10" s="1">
-        <v>60.0</v>
+        <v>80.0</v>
       </c>
       <c r="F10" s="1">
         <v>20.0</v>
@@ -634,23 +725,26 @@
       </c>
       <c r="H10" s="1">
         <v>80.0</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1">
-        <v>40.0</v>
+        <v>60.0</v>
       </c>
       <c r="C11" s="1">
-        <v>80.0</v>
+        <v>100.0</v>
       </c>
       <c r="D11" s="1">
         <v>20.0</v>
       </c>
       <c r="E11" s="1">
-        <v>80.0</v>
+        <v>60.0</v>
       </c>
       <c r="F11" s="1">
         <v>20.0</v>
@@ -659,50 +753,56 @@
         <v>60.0</v>
       </c>
       <c r="H11" s="1">
-        <v>80.0</v>
+        <v>60.0</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1">
-        <v>60.0</v>
+        <v>80.0</v>
       </c>
       <c r="C12" s="1">
-        <v>100.0</v>
+        <v>80.0</v>
       </c>
       <c r="D12" s="1">
         <v>20.0</v>
       </c>
       <c r="E12" s="1">
-        <v>60.0</v>
+        <v>40.0</v>
       </c>
       <c r="F12" s="1">
         <v>20.0</v>
       </c>
       <c r="G12" s="1">
-        <v>60.0</v>
+        <v>40.0</v>
       </c>
       <c r="H12" s="1">
-        <v>60.0</v>
+        <v>20.0</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1">
         <v>80.0</v>
       </c>
       <c r="C13" s="1">
-        <v>80.0</v>
+        <v>100.0</v>
       </c>
       <c r="D13" s="1">
         <v>20.0</v>
       </c>
       <c r="E13" s="1">
-        <v>40.0</v>
+        <v>60.0</v>
       </c>
       <c r="F13" s="1">
         <v>20.0</v>
@@ -711,47 +811,53 @@
         <v>40.0</v>
       </c>
       <c r="H13" s="1">
-        <v>20.0</v>
+        <v>40.0</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B14" s="1">
-        <v>80.0</v>
+        <v>60.0</v>
       </c>
       <c r="C14" s="1">
-        <v>100.0</v>
+        <v>40.0</v>
       </c>
       <c r="D14" s="1">
-        <v>20.0</v>
+        <v>80.0</v>
       </c>
       <c r="E14" s="1">
-        <v>60.0</v>
+        <v>80.0</v>
       </c>
       <c r="F14" s="1">
         <v>20.0</v>
       </c>
       <c r="G14" s="1">
-        <v>40.0</v>
+        <v>60.0</v>
       </c>
       <c r="H14" s="1">
-        <v>40.0</v>
+        <v>80.0</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B15" s="1">
-        <v>60.0</v>
+        <v>80.0</v>
       </c>
       <c r="C15" s="1">
-        <v>40.0</v>
+        <v>60.0</v>
       </c>
       <c r="D15" s="1">
-        <v>80.0</v>
+        <v>60.0</v>
       </c>
       <c r="E15" s="1">
         <v>80.0</v>
@@ -763,21 +869,24 @@
         <v>60.0</v>
       </c>
       <c r="H15" s="1">
-        <v>80.0</v>
+        <v>60.0</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1">
         <v>80.0</v>
       </c>
       <c r="C16" s="1">
-        <v>60.0</v>
+        <v>40.0</v>
       </c>
       <c r="D16" s="1">
-        <v>60.0</v>
+        <v>80.0</v>
       </c>
       <c r="E16" s="1">
         <v>80.0</v>
@@ -786,24 +895,27 @@
         <v>20.0</v>
       </c>
       <c r="G16" s="1">
-        <v>60.0</v>
+        <v>80.0</v>
       </c>
       <c r="H16" s="1">
-        <v>60.0</v>
+        <v>80.0</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1">
         <v>80.0</v>
       </c>
       <c r="C17" s="1">
-        <v>40.0</v>
+        <v>20.0</v>
       </c>
       <c r="D17" s="1">
-        <v>80.0</v>
+        <v>100.0</v>
       </c>
       <c r="E17" s="1">
         <v>80.0</v>
@@ -812,41 +924,47 @@
         <v>20.0</v>
       </c>
       <c r="G17" s="1">
-        <v>80.0</v>
+        <v>100.0</v>
       </c>
       <c r="H17" s="1">
-        <v>80.0</v>
+        <v>100.0</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B18" s="1">
-        <v>80.0</v>
+        <v>60.0</v>
       </c>
       <c r="C18" s="1">
-        <v>20.0</v>
+        <v>80.0</v>
       </c>
       <c r="D18" s="1">
-        <v>100.0</v>
+        <v>40.0</v>
       </c>
       <c r="E18" s="1">
-        <v>80.0</v>
+        <v>60.0</v>
       </c>
       <c r="F18" s="1">
         <v>20.0</v>
       </c>
       <c r="G18" s="1">
-        <v>100.0</v>
+        <v>60.0</v>
       </c>
       <c r="H18" s="1">
-        <v>100.0</v>
+        <v>60.0</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1">
         <v>60.0</v>
@@ -855,7 +973,7 @@
         <v>80.0</v>
       </c>
       <c r="D19" s="1">
-        <v>40.0</v>
+        <v>20.0</v>
       </c>
       <c r="E19" s="1">
         <v>60.0</v>
@@ -868,20 +986,23 @@
       </c>
       <c r="H19" s="1">
         <v>60.0</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1">
-        <v>60.0</v>
+        <v>80.0</v>
       </c>
       <c r="C20" s="1">
-        <v>80.0</v>
+        <v>60.0</v>
       </c>
       <c r="D20" s="1">
-        <v>20.0</v>
+        <v>40.0</v>
       </c>
       <c r="E20" s="1">
         <v>60.0</v>
@@ -890,18 +1011,21 @@
         <v>20.0</v>
       </c>
       <c r="G20" s="1">
-        <v>60.0</v>
+        <v>40.0</v>
       </c>
       <c r="H20" s="1">
         <v>60.0</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B21" s="1">
-        <v>80.0</v>
+        <v>60.0</v>
       </c>
       <c r="C21" s="1">
         <v>60.0</v>
@@ -910,146 +1034,106 @@
         <v>40.0</v>
       </c>
       <c r="E21" s="1">
-        <v>60.0</v>
+        <v>80.0</v>
       </c>
       <c r="F21" s="1">
         <v>20.0</v>
       </c>
       <c r="G21" s="1">
-        <v>40.0</v>
+        <v>60.0</v>
       </c>
       <c r="H21" s="1">
-        <v>60.0</v>
+        <v>80.0</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B22" s="1">
         <v>80.0</v>
       </c>
       <c r="C22" s="1">
-        <v>40.0</v>
+        <v>80.0</v>
       </c>
       <c r="D22" s="1">
         <v>60.0</v>
       </c>
       <c r="E22" s="1">
-        <v>80.0</v>
+        <v>40.0</v>
       </c>
       <c r="F22" s="1">
-        <v>80.0</v>
+        <v>20.0</v>
       </c>
       <c r="G22" s="1">
         <v>60.0</v>
       </c>
       <c r="H22" s="1">
         <v>60.0</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B23" s="1">
-        <v>60.0</v>
+        <v>80.0</v>
       </c>
       <c r="C23" s="1">
-        <v>60.0</v>
+        <v>100.0</v>
       </c>
       <c r="D23" s="1">
-        <v>40.0</v>
+        <v>60.0</v>
       </c>
       <c r="E23" s="1">
-        <v>80.0</v>
+        <v>40.0</v>
       </c>
       <c r="F23" s="1">
         <v>20.0</v>
       </c>
       <c r="G23" s="1">
-        <v>60.0</v>
+        <v>40.0</v>
       </c>
       <c r="H23" s="1">
-        <v>80.0</v>
+        <v>60.0</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="1">
-        <v>60.0</v>
-      </c>
-      <c r="C24" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="D24" s="1">
-        <v>80.0</v>
-      </c>
-      <c r="E24" s="1">
-        <v>60.0</v>
-      </c>
-      <c r="F24" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="G24" s="1">
-        <v>100.0</v>
-      </c>
-      <c r="H24" s="1">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="1">
-        <v>80.0</v>
-      </c>
-      <c r="C25" s="1">
-        <v>80.0</v>
-      </c>
-      <c r="D25" s="1">
-        <v>60.0</v>
-      </c>
-      <c r="E25" s="1">
-        <v>40.0</v>
-      </c>
-      <c r="F25" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="G25" s="1">
-        <v>60.0</v>
-      </c>
-      <c r="H25" s="1">
-        <v>60.0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="1">
-        <v>80.0</v>
-      </c>
-      <c r="C26" s="1">
-        <v>100.0</v>
-      </c>
-      <c r="D26" s="1">
-        <v>60.0</v>
-      </c>
-      <c r="E26" s="1">
-        <v>40.0</v>
-      </c>
-      <c r="F26" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="G26" s="1">
-        <v>40.0</v>
-      </c>
-      <c r="H26" s="1">
-        <v>60.0</v>
+        <v>52</v>
+      </c>
+      <c r="B24" s="2">
+        <v>70.0</v>
+      </c>
+      <c r="C24" s="2">
+        <v>60.0</v>
+      </c>
+      <c r="D24" s="2">
+        <v>90.0</v>
+      </c>
+      <c r="E24" s="2">
+        <v>60.0</v>
+      </c>
+      <c r="F24" s="2">
+        <v>20.0</v>
+      </c>
+      <c r="G24" s="2">
+        <v>40.0</v>
+      </c>
+      <c r="H24" s="2">
+        <v>40.0</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>